<commit_message>
Completed Linked List and Queue POM File, Step Definitions and Jherkins
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\git\DsAlgoPortal_CucumberBDD\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCADE96C-B91A-4241-8860-EFB08406750D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F76C5BA-6E4C-44E1-9205-6D2464A76C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -661,7 +661,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add failed scenario for Linked List and Queue
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/DsAlgo_TestData.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudhe\git\DsAlgoPortal_CucumberBDD\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09AAE9C-0EF9-4C39-9551-7AA1937A0D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Valid_Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Login" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Register" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Linked_List" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Graph" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Tree" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="TryEditor" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Array" sheetId="8" r:id="rId11"/>
+    <sheet name="Valid_Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="Linked_List" sheetId="4" r:id="rId4"/>
+    <sheet name="Graph" sheetId="5" r:id="rId5"/>
+    <sheet name="Tree" sheetId="6" r:id="rId6"/>
+    <sheet name="TryEditor" sheetId="7" r:id="rId7"/>
+    <sheet name="Array" sheetId="8" r:id="rId8"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -131,17 +140,18 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t>OutPut Result</t>
     </r>
@@ -213,16 +223,10 @@
     <t>D6947as</t>
   </si>
   <si>
-    <t>NameError: name 'D647as' is not defined on line 1</t>
-  </si>
-  <si>
     <t>$#@!&lt;&gt;</t>
   </si>
   <si>
     <t>asdfgh</t>
-  </si>
-  <si>
-    <t>NameError:name 'asdgh' is not defined on line 1</t>
   </si>
   <si>
     <t>Python Code</t>
@@ -410,87 +414,107 @@
  result = sortedSquares(nums)
  print(result) # Output: [0, 1, 9, 16, 100</t>
   </si>
+  <si>
+    <t>NameError: name 'D6947as' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>NameError: name 'asdfgh' is not defined on line 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF467886"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF467886"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="13.0"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13.0"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -499,11 +523,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -517,132 +547,66 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -832,20 +796,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="13.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -862,21 +829,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,17 +852,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="13.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="13.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="13.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -902,7 +870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="13.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -911,27 +879,28 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="18.5"/>
-    <col customWidth="1" min="3" max="3" width="19.13"/>
-    <col customWidth="1" min="4" max="4" width="34.88"/>
-    <col customWidth="1" min="5" max="5" width="50.25"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" customWidth="1"/>
+    <col min="5" max="5" width="50.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -948,7 +917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -959,9 +928,9 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="2">
-        <v>8.767686667E9</v>
+        <v>8767686667</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -970,7 +939,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -983,7 +952,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -995,7 +964,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1015,7 +984,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1035,7 +1004,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1052,7 +1021,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>21</v>
@@ -1070,7 +1039,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1089,15 +1058,15 @@
       <c r="F10" s="6"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="8">
-        <v>9.87654321E8</v>
+        <v>987654321</v>
       </c>
       <c r="C11" s="8">
-        <v>9.87654321E8</v>
+        <v>987654321</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>26</v>
@@ -1109,7 +1078,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1129,7 +1098,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1146,7 +1115,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1164,7 +1133,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1181,164 +1150,166 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="F16" s="4"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17">
+    <row r="17" spans="6:8" ht="15.75" customHeight="1">
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="6:8" ht="15.75" customHeight="1">
       <c r="F18" s="1"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19">
+    <row r="19" spans="6:8" ht="15.75" customHeight="1">
       <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20">
+    <row r="20" spans="6:8" ht="15.75" customHeight="1">
       <c r="F20" s="4"/>
       <c r="G20" s="6"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="6:8" ht="15.75" customHeight="1">
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.88"/>
-    <col customWidth="1" min="2" max="2" width="16.38"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="16.8">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" ht="30.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" ht="30.75" customHeight="1">
+      <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" ht="24.75" customHeight="1">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="24.75" customHeight="1">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="13.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="13.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="13.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="43.25"/>
-    <col customWidth="1" min="2" max="2" width="40.0"/>
+    <col min="1" max="1" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" ht="14.4">
+      <c r="A1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="13.2">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -1349,16 +1320,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="19">
-        <v>123434.0</v>
-      </c>
-      <c r="B4" s="12"/>
+    <row r="4" spans="1:3" ht="13.2">
+      <c r="A4" s="16">
+        <v>123434</v>
+      </c>
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="13.2">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -1369,7 +1340,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="13.2">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -1380,7 +1351,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="13.2">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -1391,47 +1362,48 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+    <row r="8" spans="1:3" ht="13.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="43.25"/>
-    <col customWidth="1" min="2" max="2" width="40.0"/>
+    <col min="1" max="1" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" ht="14.4">
+      <c r="A1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1">
+      <c r="A2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="18"/>
-    </row>
-    <row r="3">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="13.2">
       <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
@@ -1442,16 +1414,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="19">
-        <v>123434.0</v>
-      </c>
-      <c r="B4" s="12"/>
+    <row r="4" spans="1:3" ht="13.2">
+      <c r="A4" s="16">
+        <v>123434</v>
+      </c>
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="13.2">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -1462,7 +1434,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="13.2">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -1473,7 +1445,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="13.2">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -1484,30 +1456,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+    <row r="8" spans="1:3" ht="13.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.13"/>
-    <col customWidth="1" min="2" max="2" width="41.13"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1515,7 +1490,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1523,7 +1498,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -1531,7 +1506,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
@@ -1539,214 +1514,217 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="13.2">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13.2">
+      <c r="A6" s="2" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="13.2">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:2" ht="13.2">
+      <c r="A9" s="2">
+        <v>1234567</v>
+      </c>
       <c r="B9" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.0"/>
-    <col customWidth="1" min="2" max="2" width="40.75"/>
-    <col customWidth="1" min="3" max="3" width="41.75"/>
+    <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" customWidth="1"/>
+    <col min="3" max="3" width="41.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="23" t="s">
+      <c r="C4" s="19"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="C5" s="19"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A6" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="24"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="23" t="s">
+      <c r="B6" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="19"/>
+    </row>
+    <row r="7" spans="1:3" ht="13.2">
+      <c r="A7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="24"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="21" t="s">
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A8" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="24"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="23" t="s">
+      <c r="B8" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="24"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="23" t="s">
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A9" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B9" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="23" t="s">
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A10" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B10" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="24"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="26" t="s">
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A11" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B11" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="24"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="26" t="s">
+      <c r="C11" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="21" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A12" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="B12" s="17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="23" t="s">
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A13" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B13" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="24"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="23" t="s">
+      <c r="C13" s="19"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A14" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B14" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="24"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="23" t="s">
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A15" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="19"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A16" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="27"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="23" t="s">
+      <c r="B16" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="24"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="23" t="s">
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A17" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="24"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="24"/>
+      <c r="B17" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="19"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>